<commit_message>
Version 0.0.1 of attendance.py
</commit_message>
<xml_diff>
--- a/Attendance System.xlsx
+++ b/Attendance System.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yungng07\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yungng07\Documents\python-knowledge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF16B9C-914C-4A70-8E4D-E6641C15BF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E72F43B-79D7-4B3D-B589-6BE31D043C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DA574CEA-3384-4503-8A81-0D1E4A875DF2}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Employee ID</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Attendance</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,15 +476,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>123</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>456</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>789</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>367</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>234</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>567</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>890</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>146</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>795</v>
@@ -565,7 +565,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,15 +583,15 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>357</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>525</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>667</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>346</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>687</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>235</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>969</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>479</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>568</v>

</xml_diff>